<commit_message>
Two minor issue is solved.
</commit_message>
<xml_diff>
--- a/src/test/resources/testDataResources/DataForGroupActionSet.xlsx
+++ b/src/test/resources/testDataResources/DataForGroupActionSet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal Projects\GIT\AppiumAutomationFramework\src\test\resources\testDataResources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44235D47-8C03-48A0-A2FE-6B70023138A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF9E1381-F293-4860-B4B6-6E57135FDD21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -81,9 +81,6 @@
     <t>"Hussy"</t>
   </si>
   <si>
-    <t>"Bangladesh"</t>
-  </si>
-  <si>
     <t>"MISL"</t>
   </si>
   <si>
@@ -103,6 +100,9 @@
   </si>
   <si>
     <t>"12345678"</t>
+  </si>
+  <si>
+    <t>"Afghanistan"</t>
   </si>
 </sst>
 </file>
@@ -451,7 +451,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,7 +513,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -524,7 +524,7 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -535,7 +535,7 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -546,7 +546,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -557,7 +557,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -568,7 +568,7 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -579,7 +579,7 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -590,7 +590,7 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Android driver added insteda of Appium driver. Select value from dropdwon issue is solved. And ExtraActionIndicator column added in groupAction method.
</commit_message>
<xml_diff>
--- a/src/test/resources/testDataResources/DataForGroupActionSet.xlsx
+++ b/src/test/resources/testDataResources/DataForGroupActionSet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal Projects\GIT\AppiumAutomationFramework\src\test\resources\testDataResources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF9E1381-F293-4860-B4B6-6E57135FDD21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B26A67E-6212-4ADB-84D9-8DC0B5DA63F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
   <si>
     <t>ActionType</t>
   </si>
@@ -102,7 +102,16 @@
     <t>"12345678"</t>
   </si>
   <si>
-    <t>"Afghanistan"</t>
+    <t>ExtraActionIndicator</t>
+  </si>
+  <si>
+    <t>"NULL"</t>
+  </si>
+  <si>
+    <t>"Bangladesh"</t>
+  </si>
+  <si>
+    <t>"INSTANCENO:2"</t>
   </si>
 </sst>
 </file>
@@ -160,13 +169,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -448,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,9 +469,10 @@
     <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -471,8 +482,11 @@
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -482,8 +496,11 @@
       <c r="C2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -493,8 +510,11 @@
       <c r="C3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -504,8 +524,11 @@
       <c r="C4" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -513,10 +536,13 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -526,8 +552,11 @@
       <c r="C6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -537,8 +566,11 @@
       <c r="C7" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -548,8 +580,11 @@
       <c r="C8" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -559,8 +594,11 @@
       <c r="C9" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -570,8 +608,11 @@
       <c r="C10" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -581,8 +622,11 @@
       <c r="C11" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -591,6 +635,9 @@
       </c>
       <c r="C12" t="s">
         <v>24</v>
+      </c>
+      <c r="D12" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>